<commit_message>
feat: mejoras de flujo, UI y despliegue en Vercel
</commit_message>
<xml_diff>
--- a/files/asientos.xlsx
+++ b/files/asientos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O805"/>
+  <dimension ref="A1:P805"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,11 @@
           <t>Asientos</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Correos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2701,7 +2706,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-72714263</t>
         </is>
       </c>
     </row>
@@ -2848,7 +2853,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16733606</t>
         </is>
       </c>
     </row>
@@ -2897,7 +2902,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-40554960</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2951,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16736597</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3098,7 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-17450838</t>
         </is>
       </c>
     </row>
@@ -3235,7 +3240,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16637191</t>
         </is>
       </c>
     </row>
@@ -3328,7 +3333,7 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16562947</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3382,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-17450805</t>
         </is>
       </c>
     </row>
@@ -3426,7 +3431,7 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-17624824</t>
         </is>
       </c>
     </row>
@@ -3475,7 +3480,7 @@
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16689857</t>
         </is>
       </c>
     </row>
@@ -3524,7 +3529,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16796766</t>
         </is>
       </c>
     </row>
@@ -3612,7 +3617,7 @@
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16761556</t>
         </is>
       </c>
     </row>
@@ -5505,7 +5510,7 @@
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16761208</t>
         </is>
       </c>
       <c r="O111" t="n">
@@ -5935,7 +5940,7 @@
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-17625165</t>
         </is>
       </c>
       <c r="O120" t="n">
@@ -6161,7 +6166,7 @@
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16759780</t>
         </is>
       </c>
       <c r="O125" t="n">
@@ -6314,7 +6319,7 @@
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-43157511</t>
         </is>
       </c>
     </row>
@@ -6542,7 +6547,7 @@
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-26737638</t>
         </is>
       </c>
       <c r="O133" t="n">
@@ -6594,7 +6599,7 @@
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-40179551</t>
         </is>
       </c>
       <c r="O134" t="n">
@@ -6646,7 +6651,7 @@
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-45385378</t>
         </is>
       </c>
       <c r="O135" t="n">
@@ -9093,7 +9098,7 @@
       </c>
       <c r="M189" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-40042745</t>
         </is>
       </c>
       <c r="O189" t="n">
@@ -9585,7 +9590,7 @@
       </c>
       <c r="M199" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16729500</t>
         </is>
       </c>
       <c r="O199" t="n">
@@ -9832,7 +9837,7 @@
       </c>
       <c r="M204" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16753094</t>
         </is>
       </c>
       <c r="O204" t="n">
@@ -9988,7 +9993,7 @@
       </c>
       <c r="M207" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-43157511</t>
         </is>
       </c>
       <c r="O207" t="n">
@@ -10223,7 +10228,7 @@
       </c>
       <c r="M212" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16683457</t>
         </is>
       </c>
       <c r="O212" t="n">
@@ -10745,7 +10750,7 @@
       </c>
       <c r="M223" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-41756285</t>
         </is>
       </c>
       <c r="O223" t="n">
@@ -13029,7 +13034,7 @@
       </c>
       <c r="M274" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-7531871</t>
         </is>
       </c>
       <c r="O274" t="n">
@@ -13257,7 +13262,7 @@
       </c>
       <c r="M279" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16754694</t>
         </is>
       </c>
     </row>
@@ -13464,7 +13469,7 @@
       </c>
       <c r="M283" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16735252</t>
         </is>
       </c>
       <c r="O283" t="n">
@@ -13516,7 +13521,7 @@
       </c>
       <c r="M284" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16423762</t>
         </is>
       </c>
       <c r="O284" t="n">
@@ -13788,7 +13793,7 @@
       </c>
       <c r="M290" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16762908</t>
         </is>
       </c>
     </row>
@@ -18247,7 +18252,7 @@
       </c>
       <c r="M393" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16661452</t>
         </is>
       </c>
     </row>
@@ -18296,7 +18301,7 @@
       </c>
       <c r="M394" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16715161</t>
         </is>
       </c>
     </row>
@@ -19025,7 +19030,7 @@
       </c>
       <c r="M409" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16753094</t>
         </is>
       </c>
       <c r="O409" t="n">
@@ -19386,7 +19391,7 @@
       </c>
       <c r="M416" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16659349</t>
         </is>
       </c>
       <c r="O416" t="n">
@@ -19438,7 +19443,7 @@
       </c>
       <c r="M417" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-17631880</t>
         </is>
       </c>
       <c r="O417" t="n">
@@ -22530,7 +22535,7 @@
       </c>
       <c r="M483" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-17624824</t>
         </is>
       </c>
       <c r="O483" t="n">
@@ -22676,7 +22681,7 @@
       </c>
       <c r="M486" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-17617984</t>
         </is>
       </c>
       <c r="O486" t="n">
@@ -22728,7 +22733,7 @@
       </c>
       <c r="M487" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16715161</t>
         </is>
       </c>
       <c r="O487" t="n">
@@ -23991,7 +23996,7 @@
       </c>
       <c r="M514" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-40179551</t>
         </is>
       </c>
     </row>
@@ -24040,7 +24045,7 @@
       </c>
       <c r="M515" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-40179551</t>
         </is>
       </c>
     </row>
@@ -26223,7 +26228,7 @@
       </c>
       <c r="M564" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16754694</t>
         </is>
       </c>
     </row>
@@ -26680,7 +26685,7 @@
       </c>
       <c r="M573" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16687406</t>
         </is>
       </c>
       <c r="O573" t="n">
@@ -29229,7 +29234,7 @@
       </c>
       <c r="M629" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16683457</t>
         </is>
       </c>
       <c r="O629" t="n">
@@ -29489,7 +29494,7 @@
       </c>
       <c r="M634" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-45080863</t>
         </is>
       </c>
     </row>
@@ -29538,7 +29543,7 @@
       </c>
       <c r="M635" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-72644789</t>
         </is>
       </c>
     </row>
@@ -31475,7 +31480,7 @@
       </c>
       <c r="M677" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-43157511</t>
         </is>
       </c>
       <c r="O677" t="n">
@@ -31906,7 +31911,7 @@
       </c>
       <c r="M686" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16733606</t>
         </is>
       </c>
       <c r="O686" t="n">
@@ -32005,7 +32010,7 @@
       </c>
       <c r="M688" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-41652040</t>
         </is>
       </c>
       <c r="O688" t="n">
@@ -32443,7 +32448,7 @@
       </c>
       <c r="M697" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16702986</t>
         </is>
       </c>
       <c r="O697" t="n">
@@ -32495,7 +32500,7 @@
       </c>
       <c r="M698" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16590196</t>
         </is>
       </c>
     </row>
@@ -33155,7 +33160,7 @@
       </c>
       <c r="M712" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16722058</t>
         </is>
       </c>
       <c r="O712" t="n">
@@ -33347,7 +33352,7 @@
       </c>
       <c r="M716" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16423762</t>
         </is>
       </c>
     </row>
@@ -33396,7 +33401,7 @@
       </c>
       <c r="M717" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16722058</t>
         </is>
       </c>
       <c r="O717" t="n">
@@ -35427,7 +35432,7 @@
       </c>
       <c r="M762" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-42853214</t>
         </is>
       </c>
     </row>
@@ -36189,7 +36194,7 @@
       </c>
       <c r="M778" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16729500</t>
         </is>
       </c>
       <c r="O778" t="n">
@@ -36444,7 +36449,7 @@
       </c>
       <c r="M783" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-16761556</t>
         </is>
       </c>
       <c r="O783" t="n">
@@ -36538,7 +36543,7 @@
       </c>
       <c r="M785" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-45080863</t>
         </is>
       </c>
       <c r="O785" t="n">
@@ -36590,7 +36595,7 @@
       </c>
       <c r="M786" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-45080863</t>
         </is>
       </c>
       <c r="O786" t="n">
@@ -36827,7 +36832,7 @@
       </c>
       <c r="M791" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-26737638</t>
         </is>
       </c>
       <c r="O791" t="n">
@@ -37107,7 +37112,7 @@
       </c>
       <c r="M797" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-3701237</t>
         </is>
       </c>
       <c r="O797" t="n">
@@ -37203,7 +37208,7 @@
       </c>
       <c r="M799" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-44465574</t>
         </is>
       </c>
     </row>
@@ -37340,7 +37345,7 @@
       </c>
       <c r="M802" t="inlineStr">
         <is>
-          <t>TRABAJADOR</t>
+          <t>TRABAJADOR-71003287</t>
         </is>
       </c>
     </row>

</xml_diff>